<commit_message>
More bug fixes and rest of the logic added. Few bugs still remain.
</commit_message>
<xml_diff>
--- a/EzBilling/Files/TempBill.xlsx
+++ b/EzBilling/Files/TempBill.xlsx
@@ -23,16 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
-  <si>
-    <t>MALLIYRITYS OY</t>
-  </si>
-  <si>
-    <t>Mallintie 1</t>
-  </si>
-  <si>
-    <t>00100 Mallila</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Kuvaus</t>
   </si>
@@ -91,21 +82,12 @@
     <t>Pankki</t>
   </si>
   <si>
-    <t>Nordea</t>
-  </si>
-  <si>
     <t>Tilinumero</t>
   </si>
   <si>
-    <t>FI60 1234 5678 9012 26</t>
-  </si>
-  <si>
     <t>Swift/BIC</t>
   </si>
   <si>
-    <t>NDEAFIHH</t>
-  </si>
-  <si>
     <t>Verkkolaskut</t>
   </si>
   <si>
@@ -115,25 +97,10 @@
     <t>Arvonlisäveron ilmoittaminen</t>
   </si>
   <si>
-    <t>Mikko Mallila</t>
-  </si>
-  <si>
-    <t>Puh. 040-1234567</t>
-  </si>
-  <si>
-    <t>Sp: mikko.mallila@malliyritys.fi</t>
-  </si>
-  <si>
     <t>Työkalut</t>
   </si>
   <si>
     <t>Ostaja</t>
-  </si>
-  <si>
-    <t>Asd</t>
-  </si>
-  <si>
-    <t>ASD</t>
   </si>
 </sst>
 </file>
@@ -398,7 +365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -518,6 +485,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -531,14 +507,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1027,7 +1000,7 @@
   <dimension ref="B1:N60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1051,14 +1024,12 @@
     <row r="1" spans="2:14" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:14" ht="42.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
-      <c r="C2" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1066,9 +1037,7 @@
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
-      <c r="C3" s="26" t="s">
-        <v>1</v>
-      </c>
+      <c r="C3" s="26"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1082,20 +1051,18 @@
     </row>
     <row r="4" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-      <c r="C4" s="26" t="s">
-        <v>2</v>
-      </c>
+      <c r="C4" s="26"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="66">
+        <v>9</v>
+      </c>
+      <c r="H4" s="69">
         <f ca="1">TODAY()</f>
-        <v>41876</v>
-      </c>
-      <c r="I4" s="67"/>
+        <v>41885</v>
+      </c>
+      <c r="I4" s="70"/>
       <c r="J4" s="41"/>
       <c r="L4" s="19"/>
       <c r="M4" s="49"/>
@@ -1108,12 +1075,10 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="66">
-        <v>40954</v>
-      </c>
-      <c r="I5" s="66"/>
+        <v>13</v>
+      </c>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
       <c r="J5" s="42"/>
       <c r="L5" s="19"/>
       <c r="M5" s="1"/>
@@ -1122,82 +1087,68 @@
     <row r="6" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="51" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="35" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H6" s="35"/>
-      <c r="I6" s="35">
-        <v>1436</v>
-      </c>
+      <c r="I6" s="35"/>
       <c r="J6" s="1"/>
       <c r="L6" s="19"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="64"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="67"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
-      <c r="C7" s="26" t="s">
-        <v>35</v>
-      </c>
+      <c r="C7" s="26"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H7" s="35"/>
-      <c r="I7" s="35" t="s">
-        <v>22</v>
-      </c>
+      <c r="I7" s="35"/>
       <c r="J7" s="35"/>
       <c r="L7" s="19"/>
-      <c r="M7" s="63"/>
-      <c r="N7" s="64"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="67"/>
     </row>
     <row r="8" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
-      <c r="C8" s="26" t="s">
-        <v>36</v>
-      </c>
+      <c r="C8" s="26"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="35" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H8" s="35"/>
-      <c r="I8" s="35" t="s">
-        <v>24</v>
-      </c>
+      <c r="I8" s="35"/>
       <c r="J8" s="35"/>
       <c r="L8" s="19"/>
-      <c r="M8" s="65"/>
-      <c r="N8" s="64"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="67"/>
     </row>
     <row r="9" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
-      <c r="C9" s="26" t="s">
-        <v>36</v>
-      </c>
+      <c r="C9" s="26"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="35" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H9" s="35"/>
-      <c r="I9" s="35" t="s">
-        <v>26</v>
-      </c>
+      <c r="I9" s="35"/>
       <c r="J9" s="35"/>
       <c r="L9" s="19"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="64"/>
+      <c r="M9" s="68"/>
+      <c r="N9" s="67"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
@@ -1227,7 +1178,7 @@
     <row r="12" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1279,25 +1230,25 @@
     <row r="16" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="H16" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="38" t="s">
         <v>4</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="38" t="s">
-        <v>7</v>
       </c>
       <c r="J16" s="43"/>
     </row>
@@ -1307,7 +1258,7 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="59"/>
-      <c r="G17" s="70"/>
+      <c r="G17" s="63"/>
       <c r="H17" s="57"/>
       <c r="I17" s="55"/>
       <c r="J17" s="11"/>
@@ -1318,7 +1269,7 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="57"/>
-      <c r="G18" s="71"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="57"/>
       <c r="I18" s="55"/>
       <c r="J18" s="11"/>
@@ -1329,7 +1280,7 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="57"/>
-      <c r="G19" s="71"/>
+      <c r="G19" s="64"/>
       <c r="H19" s="57"/>
       <c r="I19" s="55"/>
       <c r="J19" s="11"/>
@@ -1340,7 +1291,7 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="57"/>
-      <c r="G20" s="71"/>
+      <c r="G20" s="64"/>
       <c r="H20" s="57"/>
       <c r="I20" s="55"/>
       <c r="J20" s="11"/>
@@ -1351,7 +1302,7 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="57"/>
-      <c r="G21" s="71"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="57"/>
       <c r="I21" s="55"/>
       <c r="J21" s="11"/>
@@ -1362,7 +1313,7 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="57"/>
-      <c r="G22" s="71"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="57"/>
       <c r="I22" s="55"/>
       <c r="J22" s="11"/>
@@ -1373,7 +1324,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="57"/>
-      <c r="G23" s="71"/>
+      <c r="G23" s="64"/>
       <c r="H23" s="57"/>
       <c r="I23" s="55"/>
       <c r="J23" s="11"/>
@@ -1384,7 +1335,7 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="57"/>
-      <c r="G24" s="71"/>
+      <c r="G24" s="64"/>
       <c r="H24" s="57"/>
       <c r="I24" s="55"/>
       <c r="J24" s="11"/>
@@ -1395,7 +1346,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="57"/>
-      <c r="G25" s="71"/>
+      <c r="G25" s="64"/>
       <c r="H25" s="57"/>
       <c r="I25" s="55"/>
       <c r="J25" s="11"/>
@@ -1406,7 +1357,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="57"/>
-      <c r="G26" s="71"/>
+      <c r="G26" s="64"/>
       <c r="H26" s="57"/>
       <c r="I26" s="55"/>
       <c r="J26" s="11"/>
@@ -1417,7 +1368,7 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="57"/>
-      <c r="G27" s="71"/>
+      <c r="G27" s="64"/>
       <c r="H27" s="57"/>
       <c r="I27" s="55"/>
       <c r="J27" s="11"/>
@@ -1428,7 +1379,7 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="57"/>
-      <c r="G28" s="71"/>
+      <c r="G28" s="64"/>
       <c r="H28" s="57"/>
       <c r="I28" s="55"/>
       <c r="J28" s="11"/>
@@ -1439,7 +1390,7 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="57"/>
-      <c r="G29" s="71"/>
+      <c r="G29" s="64"/>
       <c r="H29" s="57"/>
       <c r="I29" s="55"/>
       <c r="J29" s="11"/>
@@ -1450,7 +1401,7 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="57"/>
-      <c r="G30" s="71"/>
+      <c r="G30" s="64"/>
       <c r="H30" s="57"/>
       <c r="I30" s="55"/>
       <c r="J30" s="11"/>
@@ -1461,7 +1412,7 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="57"/>
-      <c r="G31" s="71"/>
+      <c r="G31" s="64"/>
       <c r="H31" s="57"/>
       <c r="I31" s="55"/>
       <c r="J31" s="11"/>
@@ -1472,7 +1423,7 @@
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="57"/>
-      <c r="G32" s="71"/>
+      <c r="G32" s="64"/>
       <c r="H32" s="57"/>
       <c r="I32" s="55"/>
       <c r="J32" s="11"/>
@@ -1483,7 +1434,7 @@
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="57"/>
-      <c r="G33" s="71"/>
+      <c r="G33" s="64"/>
       <c r="H33" s="57"/>
       <c r="I33" s="55"/>
       <c r="J33" s="11"/>
@@ -1494,7 +1445,7 @@
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="57"/>
-      <c r="G34" s="71"/>
+      <c r="G34" s="64"/>
       <c r="H34" s="57"/>
       <c r="I34" s="55"/>
       <c r="J34" s="11"/>
@@ -1505,7 +1456,7 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="57"/>
-      <c r="G35" s="71"/>
+      <c r="G35" s="64"/>
       <c r="H35" s="57"/>
       <c r="I35" s="55"/>
       <c r="J35" s="11"/>
@@ -1516,7 +1467,7 @@
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="57"/>
-      <c r="G36" s="71"/>
+      <c r="G36" s="64"/>
       <c r="H36" s="57"/>
       <c r="I36" s="55"/>
       <c r="J36" s="11"/>
@@ -1527,7 +1478,7 @@
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="58"/>
-      <c r="G37" s="72"/>
+      <c r="G37" s="65"/>
       <c r="H37" s="58"/>
       <c r="I37" s="56"/>
       <c r="J37" s="11"/>
@@ -1561,7 +1512,7 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="52"/>
@@ -1574,7 +1525,7 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="52"/>
@@ -1598,7 +1549,7 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="13" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H43" s="14"/>
       <c r="I43" s="53"/>
@@ -1749,57 +1700,51 @@
     </row>
     <row r="57" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="1"/>
-      <c r="C57" s="27" t="str">
+      <c r="C57" s="27">
         <f>C2</f>
-        <v>MALLIYRITYS OY</v>
-      </c>
-      <c r="D57" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
+        <v>0</v>
+      </c>
+      <c r="D57" s="74"/>
+      <c r="E57" s="74"/>
+      <c r="F57" s="74"/>
       <c r="G57" s="27"/>
-      <c r="H57" s="27" t="str">
+      <c r="H57" s="27">
         <f>I7</f>
-        <v>Nordea</v>
+        <v>0</v>
       </c>
       <c r="I57" s="20"/>
       <c r="J57" s="9"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B58" s="1"/>
-      <c r="C58" s="26" t="str">
+      <c r="C58" s="26">
         <f>C3</f>
-        <v>Mallintie 1</v>
-      </c>
-      <c r="D58" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="D58" s="73"/>
+      <c r="E58" s="73"/>
+      <c r="F58" s="73"/>
       <c r="G58" s="26"/>
-      <c r="H58" s="26" t="str">
+      <c r="H58" s="26">
         <f>I8</f>
-        <v>FI60 1234 5678 9012 26</v>
+        <v>0</v>
       </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B59" s="1"/>
-      <c r="C59" s="26" t="str">
+      <c r="C59" s="26">
         <f>C4</f>
-        <v>00100 Mallila</v>
-      </c>
-      <c r="D59" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="E59" s="26"/>
-      <c r="F59" s="26"/>
+        <v>0</v>
+      </c>
+      <c r="D59" s="73"/>
+      <c r="E59" s="73"/>
+      <c r="F59" s="73"/>
       <c r="G59" s="26"/>
-      <c r="H59" s="26" t="str">
+      <c r="H59" s="26">
         <f>I9</f>
-        <v>NDEAFIHH</v>
+        <v>0</v>
       </c>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
@@ -1816,7 +1761,10 @@
       <c r="J60" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
     <mergeCell ref="M7:N7"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="M9:N9"/>
@@ -1848,16 +1796,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="68" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
+      <c r="B1" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -1882,7 +1830,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="33" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="21"/>
@@ -1894,31 +1842,31 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="32" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D11" s="22"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="32" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D12" s="22"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="32" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D13" s="22"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="32" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D14" s="22"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="32" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D15" s="22"/>
     </row>

</xml_diff>